<commit_message>
Download fucntioning and upload functioning
</commit_message>
<xml_diff>
--- a/Links to photo.xlsx
+++ b/Links to photo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\PhotoBooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68688E79-AC30-410F-B7DE-98885FF206FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E5D027-FE6F-4B25-94C8-3B11891B3624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8014FC35-2BCF-4DBA-BCE2-72AB76053D30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>Photo Booth</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>https://img.playbook.com/LQ84wg7fMW2nYJ_04BNV4s9XTPDWvL4RUywTH0eUTFE/Z3M6Ly9wbGF5Ym9v/ay1hc3NldHMtcHVi/bGljLzNkNTViOWEw/LWE0OTctNGIzZS05/NTcwLTA0YmJkNDFk/YTkwOA</t>
+  </si>
+  <si>
+    <t>https://img.playbook.com/hnb_ls5LU1WxEF1ig9fDLEfzNyvaq4G_-N6jewhjGu4/Z3M6Ly9wbGF5Ym9v/ay1hc3NldHMtcHVi/bGljL2I5MTE0N2Vm/LTZmZGItNDUyMS1h/OTUxLTU3MjIyZmMy/Njc1Nw</t>
   </si>
 </sst>
 </file>
@@ -652,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0558D232-9DC3-42A1-8C14-EF104020A917}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +856,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>